<commit_message>
[ovsp4rt] Update FunctionsWithTests spreadsheet
Signed-off-by: Derek Foster <derek.foster@intel.com>
</commit_message>
<xml_diff>
--- a/ovs-p4rt/sidecar/testing/FunctionsWithTests.xlsx
+++ b/ovs-p4rt/sidecar/testing/FunctionsWithTests.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE5A23F-68AB-48AB-974B-E27491ADBD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF60E3E-B1D1-45CD-8CC5-18503598116E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7365" yWindow="4110" windowWidth="28800" windowHeight="15345" xr2:uid="{2D922007-F887-4B79-844A-DB4570C92912}"/>
+    <workbookView xWindow="8055" yWindow="4800" windowWidth="28800" windowHeight="15345" xr2:uid="{2D922007-F887-4B79-844A-DB4570C92912}"/>
   </bookViews>
   <sheets>
     <sheet name="Prepare Functions" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="98">
   <si>
     <t>PrepareDstIpMacMapTableEntry</t>
   </si>
@@ -300,12 +300,6 @@
   </si>
   <si>
     <t>BaseTableTest</t>
-  </si>
-  <si>
-    <t>::testing::Test</t>
-  </si>
-  <si>
-    <t>Notes</t>
   </si>
   <si>
     <t>vxlan_decap_mod_table_test</t>
@@ -321,7 +315,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,13 +456,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -657,7 +644,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -817,17 +804,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -873,15 +849,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1261,573 +1235,537 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F30">
-    <sortCondition ref="E2:E30"/>
-  </sortState>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="71" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="77" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;COVSP4RT Functions with Unit Tests</oddHeader>
+    <oddHeader>&amp;COVS-P4RT Functions with Unit Tests</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[ovsp4rt] Update FunctionsWithTests spreadsheet (#660)
Signed-off-by: Derek Foster <derek.foster@intel.com>
</commit_message>
<xml_diff>
--- a/ovs-p4rt/sidecar/testing/FunctionsWithTests.xlsx
+++ b/ovs-p4rt/sidecar/testing/FunctionsWithTests.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE5A23F-68AB-48AB-974B-E27491ADBD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF60E3E-B1D1-45CD-8CC5-18503598116E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7365" yWindow="4110" windowWidth="28800" windowHeight="15345" xr2:uid="{2D922007-F887-4B79-844A-DB4570C92912}"/>
+    <workbookView xWindow="8055" yWindow="4800" windowWidth="28800" windowHeight="15345" xr2:uid="{2D922007-F887-4B79-844A-DB4570C92912}"/>
   </bookViews>
   <sheets>
     <sheet name="Prepare Functions" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="98">
   <si>
     <t>PrepareDstIpMacMapTableEntry</t>
   </si>
@@ -300,12 +300,6 @@
   </si>
   <si>
     <t>BaseTableTest</t>
-  </si>
-  <si>
-    <t>::testing::Test</t>
-  </si>
-  <si>
-    <t>Notes</t>
   </si>
   <si>
     <t>vxlan_decap_mod_table_test</t>
@@ -321,7 +315,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,13 +456,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -657,7 +644,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -817,17 +804,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -873,15 +849,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1261,573 +1235,537 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E23" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E24" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E28" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E29" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F30">
-    <sortCondition ref="E2:E30"/>
-  </sortState>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="71" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="77" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;COVSP4RT Functions with Unit Tests</oddHeader>
+    <oddHeader>&amp;COVS-P4RT Functions with Unit Tests</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>